<commit_message>
last components added to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theba\Documents\IU\SP22\ES-SPRING-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1741313-FA26-40A1-9F4E-51DD20BF523C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417AD219-AB6B-433B-9701-31CDE2123A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="345" windowWidth="13620" windowHeight="10230" xr2:uid="{3E53ABBC-5143-4277-BE12-316733EFC8F5}"/>
+    <workbookView xWindow="1050" yWindow="195" windowWidth="13620" windowHeight="10230" xr2:uid="{3E53ABBC-5143-4277-BE12-316733EFC8F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Component Manufacturer's Part number</t>
   </si>
@@ -106,9 +106,6 @@
     <t>TestPoint</t>
   </si>
   <si>
-    <t>Conn_01x04_Male</t>
-  </si>
-  <si>
     <t>Jumper_3_Open</t>
   </si>
   <si>
@@ -118,15 +115,9 @@
     <t>TSL237S-LF</t>
   </si>
   <si>
-    <t>Conn_01x03</t>
-  </si>
-  <si>
     <t>200 R</t>
   </si>
   <si>
-    <t>STDC14</t>
-  </si>
-  <si>
     <t>STM32L432KCU6</t>
   </si>
   <si>
@@ -179,6 +170,30 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-PA3F2000V/5035883</t>
+  </si>
+  <si>
+    <t>B3B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-XH-A-LF-SN/1651046</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 3POS 2.5MM</t>
+  </si>
+  <si>
+    <t>B4B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 4POS 2.5MM</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samtec-inc/FTSH-107-01-L-DV-K/6678186</t>
+  </si>
+  <si>
+    <t>CONN HEADER SMD 14POS 1.27MM</t>
+  </si>
+  <si>
+    <t>FTSH-107-01-L-DV-K</t>
   </si>
 </sst>
 </file>
@@ -550,14 +565,14 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="71.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
   </cols>
@@ -598,13 +613,13 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>7.53</v>
@@ -617,21 +632,21 @@
         <v>7.53</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E3">
         <v>0.14000000000000001</v>
@@ -644,21 +659,21 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E4">
         <v>1.0900000000000001</v>
@@ -671,7 +686,7 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -691,13 +706,13 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E6">
         <v>3.6</v>
@@ -710,7 +725,7 @@
         <v>3.6</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -727,14 +742,29 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>0.19</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -742,7 +772,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -754,13 +784,13 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10">
         <v>1.54</v>
@@ -773,7 +803,7 @@
         <v>1.54</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -781,13 +811,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E11">
         <v>1.865</v>
@@ -814,28 +844,40 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13">
+        <v>0.21</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E14">
         <v>0.16</v>
@@ -848,19 +890,34 @@
         <v>0.32</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
         <v>29</v>
       </c>
+      <c r="E15">
+        <v>5.72</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.72</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -869,6 +926,7 @@
     <hyperlink ref="H3" r:id="rId2" xr:uid="{41C46EAD-7125-4176-A6F3-9EF61D708964}"/>
     <hyperlink ref="H6" r:id="rId3" xr:uid="{759749C7-FFBE-4740-B31B-578C92601D2C}"/>
     <hyperlink ref="H14" r:id="rId4" xr:uid="{A47173B3-8596-4168-AC8C-D42D73DF486A}"/>
+    <hyperlink ref="H15" r:id="rId5" xr:uid="{DEFE7485-3237-41DD-B5B6-4A9C65CF089F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>